<commit_message>
JaSam kup 2022, 2 etape
</commit_message>
<xml_diff>
--- a/rezultati/2022/staze.xlsx
+++ b/rezultati/2022/staze.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\file\data\Korisnici\ivo\Documents\Orijentacija\Rezultati\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Repos\orienteering-hr\rezultati\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72270D8-8AF7-44E8-B326-E6F3902C52B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5C47F2-9D2A-46BE-BDF5-C26640D0997B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{2C2F812D-F545-414D-BFB2-2A40C61ADFD4}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="55">
   <si>
     <t>M12</t>
   </si>
@@ -89,121 +89,127 @@
     <t>M20</t>
   </si>
   <si>
-    <t>OPEN</t>
-  </si>
-  <si>
-    <t>Otvorena</t>
-  </si>
-  <si>
-    <t>Ž21</t>
-  </si>
-  <si>
-    <t>M21</t>
-  </si>
-  <si>
-    <t>M 12</t>
-  </si>
-  <si>
-    <t>1.43–35–13</t>
-  </si>
-  <si>
-    <t>54–57–72–50–53–71–33–64–34–35–36–37–100––––––––––––––––</t>
-  </si>
-  <si>
-    <t>M 16</t>
-  </si>
-  <si>
-    <t>1.68–45–17</t>
-  </si>
-  <si>
-    <t>55–54–53–63–72–50–71–57–56–64–34–35–36–40–43–48–100––––––––––––</t>
-  </si>
-  <si>
-    <t>M 35</t>
-  </si>
-  <si>
-    <t>2.37–70–17</t>
-  </si>
-  <si>
-    <t>52–32–63–50–33–61–65–54–44–42–41–35–45–40–43–48–100––––––––––––</t>
-  </si>
-  <si>
-    <t>M 21</t>
-  </si>
-  <si>
-    <t>2.39–70–20</t>
-  </si>
-  <si>
-    <t>57–71–33–55–61–62–53–63–44–42–41–34–49–45–40–43–38–46–39–100–––––––––</t>
-  </si>
-  <si>
-    <t>M 45</t>
-  </si>
-  <si>
-    <t>2.02–65–16</t>
-  </si>
-  <si>
-    <t>47–53–32–55–61–63–72–50–33–64–41–46–45–37–39–100–––––––––––––</t>
-  </si>
-  <si>
-    <t>Ž 45</t>
-  </si>
-  <si>
-    <t>1.75–40–16</t>
-  </si>
-  <si>
-    <t>54–32–55–61–57–72–50–33–64–35–36–40–43–48–39–100–––––––––––––</t>
-  </si>
-  <si>
-    <t>Ž 55</t>
-  </si>
-  <si>
-    <t>1.56–40–15</t>
-  </si>
-  <si>
-    <t>52–61–65–53–50–71–54–31–55–33–64–46–36–37–100––––––––––––––</t>
-  </si>
-  <si>
-    <t>1.53–50–11</t>
-  </si>
-  <si>
-    <t>57–54–60–59–71–33–64–34–49–39–100––––––––––––––––––</t>
-  </si>
-  <si>
-    <t>Ž 16</t>
-  </si>
-  <si>
-    <t>1.53–40–12</t>
-  </si>
-  <si>
-    <t>31–54–58–59–60–71–33–64–35–46–38–100–––––––––––––––––</t>
-  </si>
-  <si>
-    <t>Ž 35</t>
-  </si>
-  <si>
-    <t>1.82–50–15</t>
-  </si>
-  <si>
-    <t>52–56–57–32–55–31–53–42–41–46–45–40–43–48–100––––––––––––––</t>
-  </si>
-  <si>
-    <t>Ž 21</t>
-  </si>
-  <si>
-    <t>2.15–70–17</t>
-  </si>
-  <si>
-    <t>47–54–71–33–61–65–62–53–63–44–41–34–49–45–37–39–100––––––––––––</t>
-  </si>
-  <si>
-    <t>Ž 65</t>
-  </si>
-  <si>
-    <t>1.2–20–13</t>
-  </si>
-  <si>
-    <t>31–54–58–50–71–32–55–33–64–34–45–38–100––––––––––––––––</t>
+    <t>M12; Ž12; Open Short</t>
+  </si>
+  <si>
+    <t>M14</t>
+  </si>
+  <si>
+    <t>M14; Ž14</t>
+  </si>
+  <si>
+    <t>M20; M35; Ž21A</t>
+  </si>
+  <si>
+    <t>M21A</t>
+  </si>
+  <si>
+    <t>M21B</t>
+  </si>
+  <si>
+    <t>M45; Ž20; Ž35</t>
+  </si>
+  <si>
+    <t>M55; Ž45</t>
+  </si>
+  <si>
+    <t>M65; M70; Ž55</t>
+  </si>
+  <si>
+    <t>M70</t>
+  </si>
+  <si>
+    <t>OPEN duga</t>
+  </si>
+  <si>
+    <t>OPEN kratka</t>
+  </si>
+  <si>
+    <t>Ž14</t>
+  </si>
+  <si>
+    <t>Ž16; Ž21B</t>
+  </si>
+  <si>
+    <t>Ž21A</t>
+  </si>
+  <si>
+    <t>Ž21B</t>
+  </si>
+  <si>
+    <t>Ž65; Ž70</t>
+  </si>
+  <si>
+    <t>Otvorena kratka</t>
+  </si>
+  <si>
+    <t>Otvorena duga</t>
+  </si>
+  <si>
+    <t>1.66–50–9</t>
+  </si>
+  <si>
+    <t>31–32–33–34–35–36–37–38–100––––––––––––––––––––</t>
+  </si>
+  <si>
+    <t>1.83–55–9</t>
+  </si>
+  <si>
+    <t>55–40–33–53–35–56–37–67–100––––––––––––––––––––</t>
+  </si>
+  <si>
+    <t>M16; M21B; Open Long</t>
+  </si>
+  <si>
+    <t>2.24–90–11</t>
+  </si>
+  <si>
+    <t>57–43–58–44–53–59–51–39–52–60–100––––––––––––––––––</t>
+  </si>
+  <si>
+    <t>57–43–58–44––59–51–39–52–60–100––––––––––––––––––</t>
+  </si>
+  <si>
+    <t>3.7–150–16</t>
+  </si>
+  <si>
+    <t>40–41–42–43–58–44–45–46–47–48–61–39–62–60–67–100–––––––––––––</t>
+  </si>
+  <si>
+    <t>4.89–220–18</t>
+  </si>
+  <si>
+    <t>40–41–42–43–44–45–46–47–48–49–50–51–39–52–53–44–54–100–––––––––––</t>
+  </si>
+  <si>
+    <t>2.82–110–11</t>
+  </si>
+  <si>
+    <t>57–40–63–62–46–61–64–47–51–45–100––––––––––––––––––</t>
+  </si>
+  <si>
+    <t>2.54–90–13</t>
+  </si>
+  <si>
+    <t>57–40–53–59–51–46–61–47–39–62–60–67–100––––––––––––––––</t>
+  </si>
+  <si>
+    <t>2.03–80–10</t>
+  </si>
+  <si>
+    <t>65–66–53–59–51–39–52–63–67–100–––––––––––––––––––</t>
+  </si>
+  <si>
+    <t>2.11–80–10</t>
+  </si>
+  <si>
+    <t>40–53–44–45–59–51–39–52–60–100–––––––––––––––––––</t>
+  </si>
+  <si>
+    <t>1.75–80–9</t>
+  </si>
+  <si>
+    <t>65–66–44–45–51–62–63–67–100––––––––––––––––––––</t>
   </si>
 </sst>
 </file>
@@ -1547,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEEAB83-7B02-4A0C-8BB0-FB5D57600EB0}">
-  <dimension ref="B2:E210"/>
+  <dimension ref="B2:E252"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C18"/>
+      <selection activeCell="B2" sqref="B2:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,58 +1569,58 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -1622,13 +1628,13 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -1636,210 +1642,266 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
         <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26"/>
@@ -2061,10 +2123,52 @@
     <row r="208" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="209" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="210" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="211" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="212" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="213" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="214" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="215" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="216" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="217" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="218" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="219" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="220" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="221" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="222" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="223" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="224" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="225" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="226" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="227" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="228" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="229" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="230" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="231" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="232" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="233" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="234" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="235" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="236" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="237" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="238" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="239" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="240" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="241" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="242" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="243" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="244" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="245" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="246" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="247" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="248" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="249" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="250" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="251" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="252" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E150">
-    <sortCondition ref="E2:E150"/>
-    <sortCondition ref="D2:D150"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E252">
+    <sortCondition ref="E2:E252"/>
+    <sortCondition ref="D2:D252"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2072,26 +2176,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE0E57E-33BF-4001-B873-4E6869674176}">
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C18"/>
+      <selection activeCell="B2" sqref="B2:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2099,16 +2203,16 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -2116,263 +2220,382 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7">
         <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
       <c r="G8" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H9">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H11">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
         <v>9</v>
       </c>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
       <c r="H12">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13">
-        <v>9</v>
-      </c>
       <c r="G13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H13">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="H14">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E15">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16">
-        <v>13</v>
-      </c>
       <c r="G16" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H16">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E17">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H17">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E18">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
         <v>15</v>
       </c>
       <c r="H18">
-        <v>17</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24">
+        <v>18</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25">
+        <v>18</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H18">
-    <sortCondition ref="E2:E18"/>
-    <sortCondition ref="H2:H18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H25">
+    <sortCondition ref="E2:E25"/>
+    <sortCondition ref="H2:H25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dodao rezultate dva dana ačkovog kupa
</commit_message>
<xml_diff>
--- a/rezultati/2022/staze.xlsx
+++ b/rezultati/2022/staze.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Repos\orienteering-hr\rezultati\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5C47F2-9D2A-46BE-BDF5-C26640D0997B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA3C7A8-4CFD-4926-B2C4-74C7F1E59EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{2C2F812D-F545-414D-BFB2-2A40C61ADFD4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{2C2F812D-F545-414D-BFB2-2A40C61ADFD4}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
   <si>
     <t>M12</t>
   </si>
@@ -89,127 +89,112 @@
     <t>M20</t>
   </si>
   <si>
-    <t>M12; Ž12; Open Short</t>
-  </si>
-  <si>
-    <t>M14</t>
-  </si>
-  <si>
-    <t>M14; Ž14</t>
-  </si>
-  <si>
-    <t>M20; M35; Ž21A</t>
-  </si>
-  <si>
-    <t>M21A</t>
-  </si>
-  <si>
-    <t>M21B</t>
-  </si>
-  <si>
-    <t>M45; Ž20; Ž35</t>
-  </si>
-  <si>
-    <t>M55; Ž45</t>
-  </si>
-  <si>
-    <t>M65; M70; Ž55</t>
-  </si>
-  <si>
-    <t>M70</t>
-  </si>
-  <si>
-    <t>OPEN duga</t>
-  </si>
-  <si>
-    <t>OPEN kratka</t>
-  </si>
-  <si>
-    <t>Ž14</t>
-  </si>
-  <si>
-    <t>Ž16; Ž21B</t>
-  </si>
-  <si>
-    <t>Ž21A</t>
-  </si>
-  <si>
-    <t>Ž21B</t>
-  </si>
-  <si>
-    <t>Ž65; Ž70</t>
-  </si>
-  <si>
-    <t>Otvorena kratka</t>
-  </si>
-  <si>
-    <t>Otvorena duga</t>
-  </si>
-  <si>
-    <t>1.66–50–9</t>
-  </si>
-  <si>
-    <t>31–32–33–34–35–36–37–38–100––––––––––––––––––––</t>
-  </si>
-  <si>
-    <t>1.83–55–9</t>
-  </si>
-  <si>
-    <t>55–40–33–53–35–56–37–67–100––––––––––––––––––––</t>
-  </si>
-  <si>
-    <t>M16; M21B; Open Long</t>
-  </si>
-  <si>
-    <t>2.24–90–11</t>
-  </si>
-  <si>
-    <t>57–43–58–44–53–59–51–39–52–60–100––––––––––––––––––</t>
-  </si>
-  <si>
-    <t>57–43–58–44––59–51–39–52–60–100––––––––––––––––––</t>
-  </si>
-  <si>
-    <t>3.7–150–16</t>
-  </si>
-  <si>
-    <t>40–41–42–43–58–44–45–46–47–48–61–39–62–60–67–100–––––––––––––</t>
-  </si>
-  <si>
-    <t>4.89–220–18</t>
-  </si>
-  <si>
-    <t>40–41–42–43–44–45–46–47–48–49–50–51–39–52–53–44–54–100–––––––––––</t>
-  </si>
-  <si>
-    <t>2.82–110–11</t>
-  </si>
-  <si>
-    <t>57–40–63–62–46–61–64–47–51–45–100––––––––––––––––––</t>
-  </si>
-  <si>
-    <t>2.54–90–13</t>
-  </si>
-  <si>
-    <t>57–40–53–59–51–46–61–47–39–62–60–67–100––––––––––––––––</t>
-  </si>
-  <si>
-    <t>2.03–80–10</t>
-  </si>
-  <si>
-    <t>65–66–53–59–51–39–52–63–67–100–––––––––––––––––––</t>
-  </si>
-  <si>
-    <t>2.11–80–10</t>
-  </si>
-  <si>
-    <t>40–53–44–45–59–51–39–52–60–100–––––––––––––––––––</t>
-  </si>
-  <si>
-    <t>1.75–80–9</t>
-  </si>
-  <si>
-    <t>65–66–44–45–51–62–63–67–100––––––––––––––––––––</t>
+    <t>M12 Ž12 OPEN</t>
+  </si>
+  <si>
+    <t>1.5–30–12</t>
+  </si>
+  <si>
+    <t>61–35–38–49–33–50–51–53–55–58–59–100–––––––––––––––––</t>
+  </si>
+  <si>
+    <t>M16 M45</t>
+  </si>
+  <si>
+    <t>2.8–50–21</t>
+  </si>
+  <si>
+    <t>37–36–35–38–39–43–44–45–46–47–49–33–61–32–50–51–53–54–57–58–100––––––––</t>
+  </si>
+  <si>
+    <t>37–36–35–38–39–43–44–45–46––49–33–61–32–50–51–53–54–57–58–100––––––––</t>
+  </si>
+  <si>
+    <t>Ž21 M35 M20</t>
+  </si>
+  <si>
+    <t>3–70–21</t>
+  </si>
+  <si>
+    <t>36–35–34–37–49–48–46–45–41–42–40–43–31–32–50–51–53–54–57–59–100––––––––</t>
+  </si>
+  <si>
+    <t>M21</t>
+  </si>
+  <si>
+    <t>3.4–70–27</t>
+  </si>
+  <si>
+    <t>31–33–34–35–36–37–38–39–40–41–42–43–44–45–46–47–48–49–50–51–52–53–54–55–57–59–100––</t>
+  </si>
+  <si>
+    <t>M55 Ž45</t>
+  </si>
+  <si>
+    <t>2.6–70–17</t>
+  </si>
+  <si>
+    <t>32–49–48–46–42–39–38–35–36–33–50–51–54–55–58–59–100––––––––––––</t>
+  </si>
+  <si>
+    <t>M65 Ž65</t>
+  </si>
+  <si>
+    <t>1.9–50–12</t>
+  </si>
+  <si>
+    <t>33–37–36–61–32–51–49–48–53–54–57–100–––––––––––––––––</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>W12</t>
+  </si>
+  <si>
+    <t>W16</t>
+  </si>
+  <si>
+    <t>Ž16 Ž55</t>
+  </si>
+  <si>
+    <t>2–50–13</t>
+  </si>
+  <si>
+    <t>34–35–37–48–47–50–51–52–53–54–55–58–100––––––––––––––––</t>
+  </si>
+  <si>
+    <t>W20</t>
+  </si>
+  <si>
+    <t>Ž20 Ž35</t>
+  </si>
+  <si>
+    <t>2.9–50–17</t>
+  </si>
+  <si>
+    <t>33–37–34–38–39–42–41–43–46–47–49–32–51–52–54–57–100––––––––––––</t>
+  </si>
+  <si>
+    <t>W21</t>
+  </si>
+  <si>
+    <t>W35</t>
+  </si>
+  <si>
+    <t>W45</t>
+  </si>
+  <si>
+    <t>W55</t>
+  </si>
+  <si>
+    <t>W65</t>
+  </si>
+  <si>
+    <t>Ž21</t>
+  </si>
+  <si>
+    <t>Otvorena</t>
   </si>
 </sst>
 </file>
@@ -1553,10 +1538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEEAB83-7B02-4A0C-8BB0-FB5D57600EB0}">
-  <dimension ref="B2:E252"/>
+  <dimension ref="B2:E233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C25"/>
+      <selection activeCell="B2" sqref="B2:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,66 +1554,66 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
         <v>41</v>
@@ -1639,114 +1624,114 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>48</v>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1754,154 +1739,106 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
         <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" t="s">
-        <v>39</v>
-      </c>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" t="s">
-        <v>40</v>
-      </c>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" t="s">
-        <v>50</v>
-      </c>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" t="s">
-        <v>50</v>
-      </c>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26"/>
@@ -2146,29 +2083,10 @@
     <row r="231" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="232" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="233" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="234" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="235" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="236" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="237" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="238" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="239" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="240" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="241" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="242" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="243" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="244" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="245" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="246" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="247" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="248" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="249" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="250" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="251" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="252" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E252">
-    <sortCondition ref="E2:E252"/>
-    <sortCondition ref="D2:D252"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E142">
+    <sortCondition ref="E2:E142"/>
+    <sortCondition ref="D2:D142"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2176,26 +2094,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE0E57E-33BF-4001-B873-4E6869674176}">
-  <dimension ref="B2:H25"/>
+  <dimension ref="B2:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C25"/>
+      <selection activeCell="B2" sqref="B2:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2203,16 +2121,16 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -2223,7 +2141,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2232,7 +2150,7 @@
         <v>2</v>
       </c>
       <c r="H4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2240,7 +2158,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2249,21 +2167,21 @@
         <v>13</v>
       </c>
       <c r="H5">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -2271,331 +2189,229 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
       <c r="G9" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="H14">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="H15">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H16">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="H17">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E18">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="H18">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E19">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="H19">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="E20">
-        <v>12</v>
-      </c>
-      <c r="G20" t="s">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21">
-        <v>12</v>
-      </c>
-      <c r="G21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22">
-        <v>12</v>
-      </c>
-      <c r="G22" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23">
-        <v>14</v>
-      </c>
-      <c r="G23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24">
-        <v>18</v>
-      </c>
-      <c r="G24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25">
-        <v>18</v>
-      </c>
-      <c r="G25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H25">
-    <sortCondition ref="E2:E25"/>
-    <sortCondition ref="H2:H25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H19">
+    <sortCondition ref="E2:E19"/>
+    <sortCondition ref="H2:H19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>